<commit_message>
Add special weapons and Dragonborn artifacts
</commit_message>
<xml_diff>
--- a/tools/Spreadsheet/Armor.xlsx
+++ b/tools/Spreadsheet/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2CEE19-A9EA-4CAA-B9B7-6A8568ABCFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F1FABE-0FC6-4D19-BDCC-A5298F3E70C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="163">
   <si>
     <t>Amber</t>
   </si>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,9 +1480,6 @@
       </c>
       <c r="D42" t="s">
         <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>1</v>
       </c>
       <c r="F42" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Standardize price of divine artifacts at 80000
</commit_message>
<xml_diff>
--- a/tools/Spreadsheet/Armor.xlsx
+++ b/tools/Spreadsheet/Armor.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002C3B5A-7B8D-4F0A-B882-57BEFF675DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC0EA8C-D22A-487F-9E8B-4AABF9CFDEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
     <sheet name="Extras" sheetId="5" r:id="rId2"/>
-    <sheet name="Stats" sheetId="4" r:id="rId3"/>
-    <sheet name="CraftingQuantities" sheetId="2" r:id="rId4"/>
-    <sheet name="Artifacts" sheetId="3" r:id="rId5"/>
+    <sheet name="CraftingQuantities" sheetId="2" r:id="rId3"/>
+    <sheet name="Artifacts" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="179">
   <si>
     <t>Amber</t>
   </si>
@@ -930,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F18:F19"/>
     </sheetView>
   </sheetViews>
@@ -2538,106 +2537,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598B841E-1A80-48A6-99E8-03FD63DEB9EB}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2">
-        <v>0.5</v>
-      </c>
-      <c r="C2">
-        <v>0.5</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
-      </c>
-      <c r="C3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4">
-        <v>0.15</v>
-      </c>
-      <c r="C4">
-        <v>0.15</v>
-      </c>
-      <c r="D4">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5">
-        <v>0.15</v>
-      </c>
-      <c r="C5">
-        <v>0.15</v>
-      </c>
-      <c r="D5">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6">
-        <v>0.3</v>
-      </c>
-      <c r="C6">
-        <v>0.25</v>
-      </c>
-      <c r="D6">
-        <v>0.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E4D632-32D4-415E-8C4D-B9628B583B19}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2729,7 +2632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -2820,7 +2723,7 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -2894,7 +2797,7 @@
         <v>130</v>
       </c>
       <c r="E21">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -3002,7 +2905,7 @@
         <v>136</v>
       </c>
       <c r="E36">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -3055,7 +2958,7 @@
         <v>50</v>
       </c>
       <c r="E40">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Group vanilla variants together
</commit_message>
<xml_diff>
--- a/tools/Spreadsheet/Armor.xlsx
+++ b/tools/Spreadsheet/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC0EA8C-D22A-487F-9E8B-4AABF9CFDEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD514016-7D98-4E36-AAAF-BA20F2F13BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,12 +598,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,13 +651,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F18:F19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,634 +1033,672 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D2">
-        <v>50000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
+        <v>250</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
-        <v>700</v>
-      </c>
-      <c r="C3">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="3">
         <v>50</v>
       </c>
-      <c r="D3">
-        <v>5000</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="D3" s="3">
+        <v>300</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
-        <v>144</v>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3">
         <v>600</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>50</v>
       </c>
-      <c r="D4">
-        <v>300</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3">
+        <v>500</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3">
+        <v>600</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3">
+        <v>500</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3">
+        <v>600</v>
+      </c>
+      <c r="C6" s="3">
         <v>50</v>
       </c>
-      <c r="B5">
-        <v>700</v>
-      </c>
-      <c r="C5">
+      <c r="D6" s="3">
+        <v>500</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3">
+        <v>600</v>
+      </c>
+      <c r="C7" s="3">
         <v>50</v>
       </c>
-      <c r="D5">
-        <v>2500</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="D7" s="3">
+        <v>500</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
-        <v>600</v>
-      </c>
-      <c r="C6">
-        <v>40</v>
-      </c>
-      <c r="D6">
-        <v>1000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7">
-        <v>1200</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7">
-        <v>50000</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
-        <v>145</v>
+      <c r="I7" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>1000</v>
       </c>
-      <c r="H8" t="s">
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4">
+        <v>700</v>
+      </c>
+      <c r="C9" s="4">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5000</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9">
+      <c r="I9" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4">
+        <v>700</v>
+      </c>
+      <c r="C10" s="4">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2500</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4">
+        <v>700</v>
+      </c>
+      <c r="C11" s="4">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4">
         <v>1000</v>
       </c>
-      <c r="C9">
-        <v>70</v>
-      </c>
-      <c r="D9">
-        <v>20000</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10">
-        <v>1200</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11">
-        <v>900</v>
-      </c>
-      <c r="C11">
-        <v>70</v>
-      </c>
-      <c r="D11">
-        <v>2000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" t="s">
-        <v>146</v>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="4">
+        <v>700</v>
+      </c>
+      <c r="C12" s="4">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4">
         <v>1000</v>
       </c>
-      <c r="C12">
-        <v>80</v>
-      </c>
-      <c r="D12">
-        <v>10000</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" t="s">
-        <v>147</v>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13">
+        <v>700</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>1500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="2">
         <v>800</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="2">
         <v>60</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="2">
         <v>400</v>
       </c>
-      <c r="H13" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="I14" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="2">
         <v>800</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="2">
         <v>60</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="2">
         <v>400</v>
       </c>
-      <c r="H14" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15">
-        <v>600</v>
-      </c>
-      <c r="C15">
-        <v>50</v>
-      </c>
-      <c r="D15">
-        <v>500</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16">
-        <v>600</v>
-      </c>
-      <c r="C16">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <v>500</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="2">
+        <v>800</v>
+      </c>
+      <c r="C16" s="2">
+        <v>60</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2">
+        <v>800</v>
+      </c>
+      <c r="C17" s="2">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2">
+        <v>800</v>
+      </c>
+      <c r="C18" s="2">
         <v>60</v>
       </c>
-      <c r="B17">
-        <v>700</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
+      <c r="D18" s="2">
         <v>1000</v>
       </c>
-      <c r="H17" t="s">
+      <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18">
-        <v>700</v>
-      </c>
-      <c r="C18">
-        <v>50</v>
-      </c>
-      <c r="D18">
-        <v>1500</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>158</v>
+      <c r="F18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19">
-        <v>500</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
-      </c>
-      <c r="D19">
-        <v>250</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" t="s">
-        <v>144</v>
+      <c r="A19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2">
+        <v>800</v>
+      </c>
+      <c r="C19" s="2">
+        <v>60</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B20">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="C20">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>10000</v>
-      </c>
-      <c r="E20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5</v>
+        <v>5000</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B21">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="C21">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D21">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22">
-        <v>800</v>
-      </c>
-      <c r="C22">
-        <v>60</v>
-      </c>
-      <c r="D22">
-        <v>1500</v>
-      </c>
-      <c r="E22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="1">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="1">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="1">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23">
+      <c r="B25" s="1">
         <v>1000</v>
       </c>
-      <c r="C23">
+      <c r="C25" s="1">
         <v>80</v>
       </c>
-      <c r="D23">
+      <c r="D25" s="1">
         <v>10000</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24">
-        <v>600</v>
-      </c>
-      <c r="C24">
-        <v>50</v>
-      </c>
-      <c r="D24">
-        <v>500</v>
-      </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25">
-        <v>800</v>
-      </c>
-      <c r="C25">
-        <v>60</v>
-      </c>
-      <c r="D25">
-        <v>1000</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B26">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D26">
-        <v>500</v>
-      </c>
-      <c r="H26" t="s">
-        <v>11</v>
+        <v>20000</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B27">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="C27">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D27">
-        <v>1000</v>
+        <v>50000</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="I27" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="B28">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D28">
-        <v>5000</v>
-      </c>
-      <c r="H28" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" t="s">
-        <v>144</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="H29" t="s">
         <v>1</v>
@@ -1610,370 +1709,372 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>550</v>
+        <v>250</v>
       </c>
       <c r="C30">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D30">
-        <v>6000</v>
+        <v>100</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31">
-        <v>350</v>
-      </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="D31">
+      <c r="A31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="5">
+        <v>300</v>
+      </c>
+      <c r="C31" s="5">
+        <v>10</v>
+      </c>
+      <c r="D31" s="5">
+        <v>300</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="5">
+        <v>300</v>
+      </c>
+      <c r="C32" s="5">
+        <v>10</v>
+      </c>
+      <c r="D32" s="5">
+        <v>200</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="5">
+        <v>300</v>
+      </c>
+      <c r="C33" s="5">
+        <v>10</v>
+      </c>
+      <c r="D33" s="5">
+        <v>200</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="5">
+        <v>300</v>
+      </c>
+      <c r="C34" s="5">
+        <v>10</v>
+      </c>
+      <c r="D34" s="5">
+        <v>200</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="5">
+        <v>300</v>
+      </c>
+      <c r="C35" s="5">
+        <v>10</v>
+      </c>
+      <c r="D35" s="5">
+        <v>200</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="5">
+        <v>300</v>
+      </c>
+      <c r="C36" s="5">
+        <v>10</v>
+      </c>
+      <c r="D36" s="5">
+        <v>200</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="5">
+        <v>300</v>
+      </c>
+      <c r="C37" s="5">
+        <v>10</v>
+      </c>
+      <c r="D37" s="5">
+        <v>200</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="5">
+        <v>300</v>
+      </c>
+      <c r="C38" s="5">
+        <v>10</v>
+      </c>
+      <c r="D38" s="5">
+        <v>200</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="5">
+        <v>300</v>
+      </c>
+      <c r="C39" s="5">
+        <v>10</v>
+      </c>
+      <c r="D39" s="5">
         <v>400</v>
       </c>
-      <c r="H31" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="5">
         <v>300</v>
       </c>
-      <c r="C32">
+      <c r="C40" s="5">
         <v>10</v>
       </c>
-      <c r="D32">
+      <c r="D40" s="5">
         <v>200</v>
       </c>
-      <c r="H32" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33">
-        <v>400</v>
-      </c>
-      <c r="C33">
-        <v>20</v>
-      </c>
-      <c r="D33">
-        <v>800</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="5">
+        <v>300</v>
+      </c>
+      <c r="C41" s="5">
         <v>10</v>
       </c>
-      <c r="I33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34">
-        <v>500</v>
-      </c>
-      <c r="C34">
-        <v>30</v>
-      </c>
-      <c r="D34">
-        <v>600</v>
-      </c>
-      <c r="H34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35">
-        <v>600</v>
-      </c>
-      <c r="C35">
-        <v>30</v>
-      </c>
-      <c r="D35">
-        <v>16000</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36">
-        <v>400</v>
-      </c>
-      <c r="C36">
-        <v>15</v>
-      </c>
-      <c r="D36">
-        <v>800</v>
-      </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37">
+      <c r="D41" s="5">
+        <v>200</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" s="5">
         <v>300</v>
       </c>
-      <c r="C37">
+      <c r="C42" s="5">
         <v>10</v>
       </c>
-      <c r="D37">
+      <c r="D42" s="5">
         <v>200</v>
       </c>
-      <c r="H37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38">
-        <v>400</v>
-      </c>
-      <c r="C38">
-        <v>20</v>
-      </c>
-      <c r="D38">
-        <v>100</v>
-      </c>
-      <c r="H38" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39">
-        <v>250</v>
-      </c>
-      <c r="C39">
-        <v>8</v>
-      </c>
-      <c r="D39">
-        <v>100</v>
-      </c>
-      <c r="H39" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40">
-        <v>250</v>
-      </c>
-      <c r="C40">
-        <v>8</v>
-      </c>
-      <c r="D40">
-        <v>100</v>
-      </c>
-      <c r="E40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41">
-        <v>550</v>
-      </c>
-      <c r="C41">
-        <v>25</v>
-      </c>
-      <c r="D41">
-        <v>6000</v>
-      </c>
-      <c r="E41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="5">
         <v>300</v>
       </c>
-      <c r="C42">
-        <v>15</v>
-      </c>
-      <c r="D42">
-        <v>400</v>
-      </c>
-      <c r="H42" t="s">
-        <v>1</v>
-      </c>
-      <c r="I42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43">
+      <c r="C43" s="5">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5">
+        <v>200</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="5">
         <v>300</v>
       </c>
-      <c r="C43">
+      <c r="C44" s="5">
         <v>10</v>
       </c>
-      <c r="D43">
+      <c r="D44" s="5">
         <v>200</v>
       </c>
-      <c r="E43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44">
-        <v>300</v>
-      </c>
-      <c r="C44">
-        <v>10</v>
-      </c>
-      <c r="D44">
-        <v>200</v>
-      </c>
-      <c r="E44" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B45">
         <v>300</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D45">
-        <v>200</v>
-      </c>
-      <c r="E45" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" t="s">
-        <v>5</v>
+        <v>400</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1</v>
       </c>
       <c r="I45" t="s">
         <v>144</v>
@@ -1981,16 +2082,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B46">
         <v>300</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D46">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H46" t="s">
         <v>1</v>
@@ -2000,152 +2101,164 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47">
-        <v>500</v>
-      </c>
-      <c r="C47">
-        <v>30</v>
-      </c>
-      <c r="D47">
+      <c r="A47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="6">
+        <v>350</v>
+      </c>
+      <c r="C47" s="6">
+        <v>12</v>
+      </c>
+      <c r="D47" s="6">
+        <v>400</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="6">
+        <v>350</v>
+      </c>
+      <c r="C48" s="6">
+        <v>12</v>
+      </c>
+      <c r="D48" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="6">
+        <v>350</v>
+      </c>
+      <c r="C49" s="6">
+        <v>12</v>
+      </c>
+      <c r="D49" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="6">
+        <v>350</v>
+      </c>
+      <c r="C50" s="6">
+        <v>12</v>
+      </c>
+      <c r="D50" s="6">
         <v>5000</v>
       </c>
-      <c r="H47" t="s">
-        <v>8</v>
-      </c>
-      <c r="I47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48">
-        <v>350</v>
-      </c>
-      <c r="C48">
-        <v>12</v>
-      </c>
-      <c r="D48">
-        <v>10000</v>
-      </c>
-      <c r="H48" t="s">
-        <v>1</v>
-      </c>
-      <c r="I48" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49">
-        <v>500</v>
-      </c>
-      <c r="C49">
-        <v>15</v>
-      </c>
-      <c r="D49">
-        <v>600</v>
-      </c>
-      <c r="H49" t="s">
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50">
-        <v>450</v>
-      </c>
-      <c r="C50">
-        <v>35</v>
-      </c>
-      <c r="D50">
-        <v>1000</v>
-      </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" t="s">
-        <v>10</v>
-      </c>
-      <c r="I50" t="s">
-        <v>159</v>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B51">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C51">
         <v>20</v>
       </c>
       <c r="D51">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I51" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B52">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="C52">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>200</v>
-      </c>
-      <c r="H52" t="s">
-        <v>1</v>
+        <v>800</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
       </c>
       <c r="I52" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B53">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D53">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I53" t="s">
         <v>144</v>
@@ -2153,65 +2266,65 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B54">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="C54">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D54">
-        <v>8000</v>
-      </c>
-      <c r="H54" t="s">
-        <v>7</v>
+        <v>1000</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
       </c>
       <c r="I54" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B55">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="C55">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D55">
-        <v>6000</v>
-      </c>
-      <c r="E55" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1</v>
-      </c>
-      <c r="G55" t="s">
-        <v>5</v>
+        <v>600</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
       </c>
       <c r="I55" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="B56">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C56">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D56">
-        <v>400</v>
+        <v>5000</v>
       </c>
       <c r="H56" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I56" t="s">
         <v>144</v>
@@ -2219,16 +2332,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B57">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C57">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D57">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="H57" t="s">
         <v>1</v>
@@ -2239,119 +2352,161 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B58">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D58">
-        <v>200</v>
-      </c>
-      <c r="H58" t="s">
-        <v>1</v>
+        <v>400</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>5</v>
       </c>
       <c r="I58" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>41</v>
       </c>
       <c r="B59">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59">
-        <v>200</v>
+        <v>8000</v>
+      </c>
+      <c r="H59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60">
-        <v>350</v>
-      </c>
-      <c r="C60">
-        <v>12</v>
-      </c>
-      <c r="D60">
-        <v>1000</v>
-      </c>
-      <c r="H60" t="s">
-        <v>1</v>
-      </c>
-      <c r="I60" t="s">
-        <v>144</v>
+      <c r="A60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="1">
+        <v>550</v>
+      </c>
+      <c r="C60" s="1">
+        <v>25</v>
+      </c>
+      <c r="D60" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61">
-        <v>350</v>
-      </c>
-      <c r="C61">
-        <v>12</v>
-      </c>
-      <c r="D61">
-        <v>5000</v>
-      </c>
-      <c r="H61" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" t="s">
-        <v>144</v>
+      <c r="A61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="1">
+        <v>550</v>
+      </c>
+      <c r="C61" s="1">
+        <v>25</v>
+      </c>
+      <c r="D61" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62">
-        <v>300</v>
-      </c>
-      <c r="C62">
-        <v>10</v>
-      </c>
-      <c r="D62">
-        <v>200</v>
-      </c>
-      <c r="H62" t="s">
-        <v>1</v>
-      </c>
-      <c r="I62" t="s">
-        <v>144</v>
+      <c r="A62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="1">
+        <v>550</v>
+      </c>
+      <c r="C62" s="1">
+        <v>25</v>
+      </c>
+      <c r="D62" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B63">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D63">
-        <v>200</v>
-      </c>
-      <c r="H63" t="s">
-        <v>1</v>
+        <v>16000</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" t="s">
+        <v>5</v>
       </c>
       <c r="I63" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:I63">
+    <sortCondition ref="B29:B63"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2540,7 +2695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E4D632-32D4-415E-8C4D-B9628B583B19}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Consistent and logical prices for artifacts
</commit_message>
<xml_diff>
--- a/tools/Spreadsheet/Armor.xlsx
+++ b/tools/Spreadsheet/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD514016-7D98-4E36-AAAF-BA20F2F13BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C5F8BE-DFAC-4888-B78B-14C28AB0E95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1536,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="1">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2791,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,7 +2832,7 @@
         <v>133</v>
       </c>
       <c r="E3">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>

</xml_diff>